<commit_message>
Add test results for dss solver with constant loads
</commit_message>
<xml_diff>
--- a/powerflowpy/tests/06n3ph_rad_unbal/06n3ph_rad_unbal_FBSvDSS.xlsx
+++ b/powerflowpy/tests/06n3ph_rad_unbal/06n3ph_rad_unbal_FBSvDSS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elainelaguerta/Dropbox/LBNL/LinDist3Flow/powerflowpy/tests/06n3ph_rad_unbal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08C7D7B7-2C7C-D64C-A60D-BB824E231A01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B6990FC-75E7-B244-AEB4-2443A9CBD9BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6320" yWindow="1760" windowWidth="28040" windowHeight="17440" activeTab="1"/>
   </bookViews>
@@ -2159,10 +2159,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>187006</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>10438</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2186,7 +2186,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317500" y="38100"/>
-          <a:ext cx="11150600" cy="22704106"/>
+          <a:ext cx="12075438" cy="24587200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2749,7 +2749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2779,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="P121" sqref="P121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add final calcs to opendss solve with constant loads
</commit_message>
<xml_diff>
--- a/powerflowpy/tests/06n3ph_rad_unbal/06n3ph_rad_unbal_FBSvDSS.xlsx
+++ b/powerflowpy/tests/06n3ph_rad_unbal/06n3ph_rad_unbal_FBSvDSS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elainelaguerta/Dropbox/LBNL/LinDist3Flow/powerflowpy/tests/06n3ph_rad_unbal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B6990FC-75E7-B244-AEB4-2443A9CBD9BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52B39E-5889-204B-A6B6-FB39A3995BDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="1760" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="6320" yWindow="1760" windowWidth="28040" windowHeight="17440" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fbs_v_dss_with_load_update" sheetId="1" r:id="rId1"/>
     <sheet name="fbs_v_dss_with_load_update_sol" sheetId="5" r:id="rId2"/>
     <sheet name="dss_w_load_update_source_code" sheetId="2" r:id="rId3"/>
-    <sheet name="fbs_source_code" sheetId="3" r:id="rId4"/>
+    <sheet name="fbs_v_dss_constant_loads" sheetId="6" r:id="rId4"/>
+    <sheet name="dss_constant_loads_source_code" sheetId="7" r:id="rId5"/>
+    <sheet name="fbs_source_code" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Input file: powerflowpy/tests/06n3ph_rad_unbal/06node_threephase_radial_unbalanced.dss</t>
   </si>
@@ -36,11 +38,17 @@
   <si>
     <t>fbs, runtime ~= 12.5ms</t>
   </si>
+  <si>
+    <t>fbs, runtime ~= 13.7 ms</t>
+  </si>
+  <si>
+    <t>dss, runtime ~= 1.32 ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1454,6 +1462,882 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>fbs vs dss_constant_loads</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fbs_v_dss_constant_loads!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fbs, runtime ~= 13.7 ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.16773425138098322"/>
+                  <c:y val="-8.8136301301437667E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fbs_v_dss_constant_loads!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fbs_v_dss_constant_loads!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>19.5488369999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.2524039999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.739209999999801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.633386000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.934189000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73.072042999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.772569999999803</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.521090000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>109.093659</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>122.14632400000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>132.56440699999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149.71262999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>166.133051999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>175.10452899999899</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>188.52859900000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>218.22581799999901</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>247.202125999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>238.87371399999901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>226.898573</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>311.52812799999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6984-8C43-B803-69511F975C81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fbs_v_dss_constant_loads!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dss, runtime ~= 1.32 ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.16531087317829923"/>
+                  <c:y val="-1.2624944373302818E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fbs_v_dss_constant_loads!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fbs_v_dss_constant_loads!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.833313</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.70719799999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9515730000000402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1188389999999799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9682620000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.07859199999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0433149999999891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.691251999999899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.488398</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.214974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.079432000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.5810969999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.998960999999898</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.008322999999901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.400048999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.628178999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.4661709999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.367904999999901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.566180000000099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28.152240999999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6984-8C43-B803-69511F975C81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1266523311"/>
+        <c:axId val="1266509103"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1266523311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>number of times solved</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1266509103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1266509103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Runtime, ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1266523311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.71527865313600747"/>
+          <c:y val="0.35331739186985367"/>
+          <c:w val="0.25863259734398197"/>
+          <c:h val="0.29069013432144508"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1494,7 +2378,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2150,6 +3590,49 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57E236C-7B1C-5847-882C-916B953D17C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2494,7 +3977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2746,10 +4229,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+    <sheetView topLeftCell="A84" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2761,7 +4244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2776,7 +4259,273 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8B2778-06D8-4042-A4DA-84A8BAED8781}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>19.5488369999998</v>
+      </c>
+      <c r="C3">
+        <v>1.833313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>36.2524039999998</v>
+      </c>
+      <c r="C4">
+        <v>2.70719799999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>41.739209999999801</v>
+      </c>
+      <c r="C5">
+        <v>3.9515730000000402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>49.633386000000002</v>
+      </c>
+      <c r="C6">
+        <v>5.1188389999999799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>59.934189000000003</v>
+      </c>
+      <c r="C7">
+        <v>6.9682620000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>73.072042999999994</v>
+      </c>
+      <c r="C8">
+        <v>8.07859199999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>83.772569999999803</v>
+      </c>
+      <c r="C9">
+        <v>9.0433149999999891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>95.521090000000001</v>
+      </c>
+      <c r="C10">
+        <v>10.691251999999899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>109.093659</v>
+      </c>
+      <c r="C11">
+        <v>11.488398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>122.14632400000001</v>
+      </c>
+      <c r="C12">
+        <v>13.214974</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>132.56440699999999</v>
+      </c>
+      <c r="C13">
+        <v>14.079432000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>149.71262999999999</v>
+      </c>
+      <c r="C14">
+        <v>16.5810969999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>166.133051999999</v>
+      </c>
+      <c r="C15">
+        <v>16.998960999999898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>175.10452899999899</v>
+      </c>
+      <c r="C16">
+        <v>18.008322999999901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>188.52859900000001</v>
+      </c>
+      <c r="C17">
+        <v>19.400048999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>218.22581799999901</v>
+      </c>
+      <c r="C18">
+        <v>20.628178999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>247.202125999999</v>
+      </c>
+      <c r="C19">
+        <v>22.4661709999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>238.87371399999901</v>
+      </c>
+      <c r="C20">
+        <v>23.367904999999901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>226.898573</v>
+      </c>
+      <c r="C21">
+        <v>24.566180000000099</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>311.52812799999998</v>
+      </c>
+      <c r="C22">
+        <v>28.152240999999901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8295BAF-8795-B948-BFF3-2AF042415402}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">

</xml_diff>